<commit_message>
updsated racp, bgdpbes, csc, raf, rqsd, bfpat
</commit_message>
<xml_diff>
--- a/InputData/ctrl-settings/RACP/RPS Alternative Compliance Payment.xlsx
+++ b/InputData/ctrl-settings/RACP/RPS Alternative Compliance Payment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\ctrl-settings\RACP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olivia Ashmoore\Documents\EPS_Models by Region\RMI\RMI_all_states\WY\ctrl-settings\RACP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40486EA8-A6B9-4E6F-AA87-67D8340A717A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8FB9CD74-6B5A-4C96-95FE-E2F691F538D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{987F1A2C-D0FF-46D7-8396-B08F06D764BF}"/>
+    <workbookView xWindow="335" yWindow="375" windowWidth="14400" windowHeight="7455" xr2:uid="{987F1A2C-D0FF-46D7-8396-B08F06D764BF}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Source:</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>2021 dollars per 2012 dollar</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
   </si>
 </sst>
 </file>
@@ -110,9 +113,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,20 +431,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAF84CE-31BD-44F2-91E9-58D4BA5F9B1E}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2">
+        <v>45363</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,7 +458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -456,22 +466,22 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.75">
       <c r="B9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.75">
       <c r="A11">
         <v>0.84730412960844359</v>
       </c>
@@ -495,20 +505,20 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
-        <f>100/About!A11</f>
-        <v>118.02137686524911</v>
+        <f>ROUND(100/About!A11,0)</f>
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>